<commit_message>
feat: Added GBR, BOM, CPL files for the project
</commit_message>
<xml_diff>
--- a/CubeSat_HW/CubeSAT_Power/Gerbers_Power/BOM.xlsx
+++ b/CubeSat_HW/CubeSAT_Power/Gerbers_Power/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\CubeSat\CubeSat_HW\CubeSAT_Power\Gerbers_Power\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CA1131-252E-49B4-B863-439F748C274E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9966EDE-BDA9-462C-9D89-6B4FE6AAE5EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Comment</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Q3</t>
   </si>
   <si>
-    <t>J4</t>
-  </si>
-  <si>
     <t>Q2</t>
   </si>
   <si>
@@ -147,13 +144,25 @@
     <t>C21190</t>
   </si>
   <si>
-    <t>C725892</t>
-  </si>
-  <si>
     <t>C8545</t>
   </si>
   <si>
     <t>C7171</t>
+  </si>
+  <si>
+    <t>C79866</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>Micro USB</t>
+  </si>
+  <si>
+    <t>C381144</t>
+  </si>
+  <si>
+    <t>J3</t>
   </si>
 </sst>
 </file>
@@ -612,18 +621,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="26" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1">
@@ -651,7 +660,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
@@ -665,26 +674,26 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>11</v>
@@ -693,26 +702,26 @@
         <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>13</v>
@@ -721,35 +730,49 @@
         <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Added Payload Board and new Gerbers for the project
</commit_message>
<xml_diff>
--- a/CubeSat_HW/CubeSAT_Power/Gerbers_Power/BOM.xlsx
+++ b/CubeSat_HW/CubeSAT_Power/Gerbers_Power/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\CubeSat\CubeSat_HW\CubeSAT_Power\Gerbers_Power\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9966EDE-BDA9-462C-9D89-6B4FE6AAE5EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BCC6A0-E1EB-423C-94AD-8B5D99158A3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="48" windowWidth="23016" windowHeight="12192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Comment</t>
   </si>
@@ -126,21 +126,9 @@
     <t>10uF</t>
   </si>
   <si>
-    <t>IRLM2502</t>
-  </si>
-  <si>
-    <t>Conn_02x20_Odd_Even</t>
-  </si>
-  <si>
-    <t>PinHeader_2x20_P2.54mm_Vertical</t>
-  </si>
-  <si>
     <t>2N7002</t>
   </si>
   <si>
-    <t>C347503</t>
-  </si>
-  <si>
     <t>C21190</t>
   </si>
   <si>
@@ -150,9 +138,6 @@
     <t>C7171</t>
   </si>
   <si>
-    <t>C79866</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -162,7 +147,10 @@
     <t>C381144</t>
   </si>
   <si>
-    <t>J3</t>
+    <t>IRLM6402</t>
+  </si>
+  <si>
+    <t>C347504</t>
   </si>
 </sst>
 </file>
@@ -621,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -702,7 +690,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
@@ -716,12 +704,12 @@
         <v>21</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>13</v>
@@ -730,49 +718,35 @@
         <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>